<commit_message>
added new results file
</commit_message>
<xml_diff>
--- a/results/6c16g.xlsx
+++ b/results/6c16g.xlsx
@@ -13,8 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Region height" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId3"/>
+  </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Nodes</t>
   </si>
@@ -67,6 +72,24 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Relative performance</t>
+  </si>
+  <si>
+    <t>Absolute performance</t>
+  </si>
+  <si>
+    <t>Minimum time</t>
+  </si>
 </sst>
 </file>
 
@@ -102,8 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,6 +146,1270 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Grzegorz Gurgul" refreshedDate="42905.931730902776" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="67">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:N1048576" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="14">
+    <cacheField name="Nodes" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Problem size" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="6144" maxValue="6144"/>
+    </cacheField>
+    <cacheField name="Steps" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Max batch size" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="26"/>
+    </cacheField>
+    <cacheField name="Batch ratio" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Region height" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="11" count="12">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Creation" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="6992" maxValue="26625"/>
+    </cacheField>
+    <cacheField name="Initialization" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="72835" maxValue="84267"/>
+    </cacheField>
+    <cacheField name="Factorization" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3943" maxValue="19835"/>
+    </cacheField>
+    <cacheField name="Backwards substitution" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="6039" maxValue="35624"/>
+    </cacheField>
+    <cacheField name="Solution reading" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2048" maxValue="3671"/>
+    </cacheField>
+    <cacheField name="First stage total" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="76906" maxValue="111145"/>
+    </cacheField>
+    <cacheField name="Second stage total" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="16641" maxValue="48776"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="94752" maxValue="159921"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="67">
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18776"/>
+    <n v="78579"/>
+    <n v="14348"/>
+    <n v="23350"/>
+    <n v="2644"/>
+    <n v="99242"/>
+    <n v="38712"/>
+    <n v="137954"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18156"/>
+    <n v="78863"/>
+    <n v="14270"/>
+    <n v="22357"/>
+    <n v="2424"/>
+    <n v="99662"/>
+    <n v="36672"/>
+    <n v="136334"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18850"/>
+    <n v="77779"/>
+    <n v="13780"/>
+    <n v="23097"/>
+    <n v="2904"/>
+    <n v="100474"/>
+    <n v="36184"/>
+    <n v="136658"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18409"/>
+    <n v="77340"/>
+    <n v="13708"/>
+    <n v="22050"/>
+    <n v="2104"/>
+    <n v="98511"/>
+    <n v="35307"/>
+    <n v="133818"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="18413"/>
+    <n v="76701"/>
+    <n v="13813"/>
+    <n v="22015"/>
+    <n v="2703"/>
+    <n v="98540"/>
+    <n v="35358"/>
+    <n v="133898"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="17737"/>
+    <n v="77234"/>
+    <n v="13715"/>
+    <n v="21933"/>
+    <n v="2419"/>
+    <n v="97960"/>
+    <n v="35312"/>
+    <n v="133272"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="9537"/>
+    <n v="75554"/>
+    <n v="7018"/>
+    <n v="10452"/>
+    <n v="2280"/>
+    <n v="83368"/>
+    <n v="21682"/>
+    <n v="105050"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="10911"/>
+    <n v="77197"/>
+    <n v="7206"/>
+    <n v="11776"/>
+    <n v="2258"/>
+    <n v="85455"/>
+    <n v="24110"/>
+    <n v="109565"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="10798"/>
+    <n v="77929"/>
+    <n v="7333"/>
+    <n v="11556"/>
+    <n v="2331"/>
+    <n v="87139"/>
+    <n v="23071"/>
+    <n v="110210"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="10122"/>
+    <n v="78196"/>
+    <n v="6951"/>
+    <n v="11723"/>
+    <n v="2512"/>
+    <n v="86579"/>
+    <n v="23131"/>
+    <n v="109710"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="10460"/>
+    <n v="77599"/>
+    <n v="7235"/>
+    <n v="11644"/>
+    <n v="2837"/>
+    <n v="86355"/>
+    <n v="23637"/>
+    <n v="109992"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="1"/>
+    <n v="10817"/>
+    <n v="77194"/>
+    <n v="7452"/>
+    <n v="11330"/>
+    <n v="2859"/>
+    <n v="86523"/>
+    <n v="23354"/>
+    <n v="109877"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="9054"/>
+    <n v="80555"/>
+    <n v="5522"/>
+    <n v="8543"/>
+    <n v="2364"/>
+    <n v="86497"/>
+    <n v="19721"/>
+    <n v="106218"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="10355"/>
+    <n v="81715"/>
+    <n v="5677"/>
+    <n v="10187"/>
+    <n v="2678"/>
+    <n v="88345"/>
+    <n v="22474"/>
+    <n v="110819"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="10560"/>
+    <n v="82253"/>
+    <n v="5728"/>
+    <n v="9668"/>
+    <n v="2565"/>
+    <n v="89331"/>
+    <n v="21724"/>
+    <n v="111055"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="10341"/>
+    <n v="81536"/>
+    <n v="6109"/>
+    <n v="10297"/>
+    <n v="2370"/>
+    <n v="88768"/>
+    <n v="22074"/>
+    <n v="110842"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="10299"/>
+    <n v="81477"/>
+    <n v="5963"/>
+    <n v="9564"/>
+    <n v="2244"/>
+    <n v="87791"/>
+    <n v="22009"/>
+    <n v="109800"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="2"/>
+    <n v="10255"/>
+    <n v="81498"/>
+    <n v="5641"/>
+    <n v="9799"/>
+    <n v="2824"/>
+    <n v="88418"/>
+    <n v="21853"/>
+    <n v="110271"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="7447"/>
+    <n v="73443"/>
+    <n v="4661"/>
+    <n v="6767"/>
+    <n v="2268"/>
+    <n v="76906"/>
+    <n v="17846"/>
+    <n v="94752"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="7934"/>
+    <n v="75209"/>
+    <n v="4671"/>
+    <n v="7807"/>
+    <n v="2482"/>
+    <n v="80243"/>
+    <n v="18041"/>
+    <n v="98284"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="8819"/>
+    <n v="74610"/>
+    <n v="5493"/>
+    <n v="9127"/>
+    <n v="2954"/>
+    <n v="81744"/>
+    <n v="19460"/>
+    <n v="101204"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="8365"/>
+    <n v="76862"/>
+    <n v="4926"/>
+    <n v="7939"/>
+    <n v="3639"/>
+    <n v="83004"/>
+    <n v="18959"/>
+    <n v="101963"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="8532"/>
+    <n v="76087"/>
+    <n v="5259"/>
+    <n v="8554"/>
+    <n v="2360"/>
+    <n v="81148"/>
+    <n v="19847"/>
+    <n v="100995"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="3"/>
+    <n v="8599"/>
+    <n v="76743"/>
+    <n v="4840"/>
+    <n v="8419"/>
+    <n v="2431"/>
+    <n v="81014"/>
+    <n v="20201"/>
+    <n v="101215"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="9468"/>
+    <n v="74610"/>
+    <n v="6055"/>
+    <n v="9364"/>
+    <n v="2509"/>
+    <n v="81377"/>
+    <n v="20815"/>
+    <n v="102192"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="10349"/>
+    <n v="77421"/>
+    <n v="6565"/>
+    <n v="10349"/>
+    <n v="2548"/>
+    <n v="84751"/>
+    <n v="22663"/>
+    <n v="107414"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="11201"/>
+    <n v="77652"/>
+    <n v="6708"/>
+    <n v="10481"/>
+    <n v="2714"/>
+    <n v="85735"/>
+    <n v="23242"/>
+    <n v="108977"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="12109"/>
+    <n v="76568"/>
+    <n v="7149"/>
+    <n v="11424"/>
+    <n v="2451"/>
+    <n v="85965"/>
+    <n v="23959"/>
+    <n v="109924"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="12006"/>
+    <n v="77836"/>
+    <n v="6786"/>
+    <n v="12435"/>
+    <n v="2048"/>
+    <n v="87137"/>
+    <n v="24176"/>
+    <n v="111313"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="4"/>
+    <n v="11748"/>
+    <n v="76883"/>
+    <n v="7099"/>
+    <n v="11362"/>
+    <n v="2115"/>
+    <n v="85853"/>
+    <n v="23581"/>
+    <n v="109434"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="6992"/>
+    <n v="82339"/>
+    <n v="3943"/>
+    <n v="6039"/>
+    <n v="2510"/>
+    <n v="85359"/>
+    <n v="16641"/>
+    <n v="102000"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="7391"/>
+    <n v="81185"/>
+    <n v="4638"/>
+    <n v="6245"/>
+    <n v="2515"/>
+    <n v="85040"/>
+    <n v="17101"/>
+    <n v="102141"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="8686"/>
+    <n v="81169"/>
+    <n v="4865"/>
+    <n v="7282"/>
+    <n v="3410"/>
+    <n v="86274"/>
+    <n v="19306"/>
+    <n v="105580"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="9105"/>
+    <n v="82396"/>
+    <n v="5624"/>
+    <n v="8288"/>
+    <n v="3006"/>
+    <n v="87451"/>
+    <n v="21127"/>
+    <n v="108578"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="9206"/>
+    <n v="83676"/>
+    <n v="6476"/>
+    <n v="7684"/>
+    <n v="2654"/>
+    <n v="89110"/>
+    <n v="20792"/>
+    <n v="109902"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="5"/>
+    <n v="9515"/>
+    <n v="84267"/>
+    <n v="5756"/>
+    <n v="8789"/>
+    <n v="3671"/>
+    <n v="89830"/>
+    <n v="22309"/>
+    <n v="112139"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="7287"/>
+    <n v="76873"/>
+    <n v="4991"/>
+    <n v="6069"/>
+    <n v="2288"/>
+    <n v="79812"/>
+    <n v="17865"/>
+    <n v="97677"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="8147"/>
+    <n v="77064"/>
+    <n v="4726"/>
+    <n v="7454"/>
+    <n v="3048"/>
+    <n v="82090"/>
+    <n v="18558"/>
+    <n v="100648"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="8583"/>
+    <n v="77655"/>
+    <n v="4876"/>
+    <n v="8223"/>
+    <n v="2316"/>
+    <n v="83140"/>
+    <n v="18688"/>
+    <n v="101828"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="9272"/>
+    <n v="77735"/>
+    <n v="6513"/>
+    <n v="8155"/>
+    <n v="3439"/>
+    <n v="83490"/>
+    <n v="21822"/>
+    <n v="105312"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="9347"/>
+    <n v="78791"/>
+    <n v="5479"/>
+    <n v="9746"/>
+    <n v="2756"/>
+    <n v="85533"/>
+    <n v="20761"/>
+    <n v="106294"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="6"/>
+    <n v="9578"/>
+    <n v="77382"/>
+    <n v="6293"/>
+    <n v="9876"/>
+    <n v="3093"/>
+    <n v="84531"/>
+    <n v="21870"/>
+    <n v="106401"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="8708"/>
+    <n v="72835"/>
+    <n v="5446"/>
+    <n v="8038"/>
+    <n v="2108"/>
+    <n v="78341"/>
+    <n v="18958"/>
+    <n v="97299"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="9977"/>
+    <n v="75204"/>
+    <n v="5725"/>
+    <n v="9311"/>
+    <n v="2633"/>
+    <n v="82138"/>
+    <n v="20896"/>
+    <n v="103034"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="10043"/>
+    <n v="73973"/>
+    <n v="6040"/>
+    <n v="9630"/>
+    <n v="2560"/>
+    <n v="80859"/>
+    <n v="21572"/>
+    <n v="102431"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="10326"/>
+    <n v="76497"/>
+    <n v="6473"/>
+    <n v="10227"/>
+    <n v="2455"/>
+    <n v="83391"/>
+    <n v="22754"/>
+    <n v="106145"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="10776"/>
+    <n v="75788"/>
+    <n v="6959"/>
+    <n v="10331"/>
+    <n v="2465"/>
+    <n v="83820"/>
+    <n v="22695"/>
+    <n v="106515"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="7"/>
+    <n v="10891"/>
+    <n v="75376"/>
+    <n v="6998"/>
+    <n v="10973"/>
+    <n v="2375"/>
+    <n v="82855"/>
+    <n v="23960"/>
+    <n v="106815"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="12325"/>
+    <n v="78824"/>
+    <n v="7915"/>
+    <n v="10633"/>
+    <n v="2578"/>
+    <n v="88305"/>
+    <n v="24130"/>
+    <n v="112435"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="13096"/>
+    <n v="79622"/>
+    <n v="8517"/>
+    <n v="12993"/>
+    <n v="2518"/>
+    <n v="90973"/>
+    <n v="25966"/>
+    <n v="116939"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="14178"/>
+    <n v="80601"/>
+    <n v="8358"/>
+    <n v="14285"/>
+    <n v="2467"/>
+    <n v="92627"/>
+    <n v="27448"/>
+    <n v="120075"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="13966"/>
+    <n v="80011"/>
+    <n v="8770"/>
+    <n v="13858"/>
+    <n v="2362"/>
+    <n v="92024"/>
+    <n v="27155"/>
+    <n v="119179"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="14248"/>
+    <n v="80920"/>
+    <n v="8673"/>
+    <n v="15492"/>
+    <n v="2432"/>
+    <n v="93762"/>
+    <n v="28201"/>
+    <n v="121963"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="8"/>
+    <n v="14170"/>
+    <n v="79855"/>
+    <n v="8933"/>
+    <n v="16047"/>
+    <n v="2420"/>
+    <n v="92864"/>
+    <n v="28765"/>
+    <n v="121629"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="14897"/>
+    <n v="73320"/>
+    <n v="11187"/>
+    <n v="15741"/>
+    <n v="2298"/>
+    <n v="88918"/>
+    <n v="28681"/>
+    <n v="117599"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="15969"/>
+    <n v="75377"/>
+    <n v="10732"/>
+    <n v="16937"/>
+    <n v="2391"/>
+    <n v="91266"/>
+    <n v="30324"/>
+    <n v="121590"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="16535"/>
+    <n v="76128"/>
+    <n v="10795"/>
+    <n v="18656"/>
+    <n v="2140"/>
+    <n v="93129"/>
+    <n v="31287"/>
+    <n v="124416"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="17241"/>
+    <n v="75233"/>
+    <n v="11424"/>
+    <n v="21284"/>
+    <n v="2374"/>
+    <n v="94544"/>
+    <n v="33177"/>
+    <n v="127721"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="18084"/>
+    <n v="74601"/>
+    <n v="11284"/>
+    <n v="22024"/>
+    <n v="2770"/>
+    <n v="94858"/>
+    <n v="34058"/>
+    <n v="128916"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="9"/>
+    <n v="18903"/>
+    <n v="75283"/>
+    <n v="11532"/>
+    <n v="21791"/>
+    <n v="2218"/>
+    <n v="95788"/>
+    <n v="34098"/>
+    <n v="129886"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="23636"/>
+    <n v="73252"/>
+    <n v="17821"/>
+    <n v="26870"/>
+    <n v="2098"/>
+    <n v="102339"/>
+    <n v="41497"/>
+    <n v="143837"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="6"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="23979"/>
+    <n v="75000"/>
+    <n v="18177"/>
+    <n v="29030"/>
+    <n v="2139"/>
+    <n v="105168"/>
+    <n v="43304"/>
+    <n v="148472"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="11"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="24862"/>
+    <n v="75140"/>
+    <n v="17749"/>
+    <n v="31453"/>
+    <n v="2207"/>
+    <n v="106108"/>
+    <n v="45457"/>
+    <n v="151565"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="16"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="25650"/>
+    <n v="74774"/>
+    <n v="18627"/>
+    <n v="33022"/>
+    <n v="2440"/>
+    <n v="107733"/>
+    <n v="46953"/>
+    <n v="154686"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="21"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="26426"/>
+    <n v="75731"/>
+    <n v="19382"/>
+    <n v="35260"/>
+    <n v="2323"/>
+    <n v="110521"/>
+    <n v="48752"/>
+    <n v="159273"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <n v="6144"/>
+    <n v="1"/>
+    <n v="26"/>
+    <n v="1"/>
+    <x v="10"/>
+    <n v="26625"/>
+    <n v="75580"/>
+    <n v="19835"/>
+    <n v="35624"/>
+    <n v="2116"/>
+    <n v="111145"/>
+    <n v="48776"/>
+    <n v="159921"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:A14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q1048576" totalsRowShown="0">
+  <autoFilter ref="A1:Q1048576"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Nodes"/>
+    <tableColumn id="2" name="Problem size"/>
+    <tableColumn id="3" name="Steps"/>
+    <tableColumn id="4" name="Max batch size"/>
+    <tableColumn id="5" name="Batch ratio"/>
+    <tableColumn id="6" name="Region height"/>
+    <tableColumn id="7" name="Creation"/>
+    <tableColumn id="8" name="Initialization"/>
+    <tableColumn id="9" name="Factorization"/>
+    <tableColumn id="10" name="Backwards substitution"/>
+    <tableColumn id="11" name="Solution reading"/>
+    <tableColumn id="12" name="First stage total"/>
+    <tableColumn id="13" name="Second stage total"/>
+    <tableColumn id="14" name="Total"/>
+    <tableColumn id="15" name="Minimum time"/>
+    <tableColumn id="16" name="Relative performance"/>
+    <tableColumn id="17" name="Absolute performance"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,29 +1675,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +1743,17 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -493,8 +1796,12 @@
       <c r="N2">
         <v>137954</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -537,8 +1844,12 @@
       <c r="N3">
         <v>136334</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -581,8 +1892,12 @@
       <c r="N4">
         <v>136658</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -625,8 +1940,12 @@
       <c r="N5">
         <v>133818</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -669,8 +1988,12 @@
       <c r="N6">
         <v>133898</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -713,8 +2036,12 @@
       <c r="N7">
         <v>133272</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -757,8 +2084,12 @@
       <c r="N8">
         <v>105050</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -801,8 +2132,12 @@
       <c r="N9">
         <v>109565</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -845,8 +2180,12 @@
       <c r="N10">
         <v>110210</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -889,8 +2228,12 @@
       <c r="N11">
         <v>109710</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -933,8 +2276,12 @@
       <c r="N12">
         <v>109992</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -977,8 +2324,12 @@
       <c r="N13">
         <v>109877</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1021,8 +2372,12 @@
       <c r="N14">
         <v>106218</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1065,8 +2420,12 @@
       <c r="N15">
         <v>110819</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1109,8 +2468,12 @@
       <c r="N16">
         <v>111055</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1153,8 +2516,12 @@
       <c r="N17">
         <v>110842</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1197,8 +2564,12 @@
       <c r="N18">
         <v>109800</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1241,8 +2612,12 @@
       <c r="N19">
         <v>110271</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1285,8 +2660,12 @@
       <c r="N20">
         <v>94752</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1329,8 +2708,12 @@
       <c r="N21">
         <v>98284</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1373,8 +2756,12 @@
       <c r="N22">
         <v>101204</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1417,8 +2804,12 @@
       <c r="N23">
         <v>101963</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1461,8 +2852,12 @@
       <c r="N24">
         <v>100995</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1505,8 +2900,12 @@
       <c r="N25">
         <v>101215</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1549,8 +2948,12 @@
       <c r="N26">
         <v>102192</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1593,8 +2996,12 @@
       <c r="N27">
         <v>107414</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1637,8 +3044,12 @@
       <c r="N28">
         <v>108977</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1681,8 +3092,12 @@
       <c r="N29">
         <v>109924</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1725,8 +3140,12 @@
       <c r="N30">
         <v>111313</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1769,8 +3188,12 @@
       <c r="N31">
         <v>109434</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1813,8 +3236,12 @@
       <c r="N32">
         <v>102000</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1857,8 +3284,12 @@
       <c r="N33">
         <v>102141</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1901,8 +3332,12 @@
       <c r="N34">
         <v>105580</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1945,8 +3380,12 @@
       <c r="N35">
         <v>108578</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1989,8 +3428,12 @@
       <c r="N36">
         <v>109902</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2033,8 +3476,12 @@
       <c r="N37">
         <v>112139</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2077,8 +3524,12 @@
       <c r="N38">
         <v>97677</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2121,8 +3572,12 @@
       <c r="N39">
         <v>100648</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2165,8 +3620,12 @@
       <c r="N40">
         <v>101828</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2209,8 +3668,12 @@
       <c r="N41">
         <v>105312</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2253,8 +3716,12 @@
       <c r="N42">
         <v>106294</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2297,8 +3764,12 @@
       <c r="N43">
         <v>106401</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2341,8 +3812,12 @@
       <c r="N44">
         <v>97299</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2385,8 +3860,12 @@
       <c r="N45">
         <v>103034</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -2429,8 +3908,12 @@
       <c r="N46">
         <v>102431</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2473,8 +3956,12 @@
       <c r="N47">
         <v>106145</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4</v>
       </c>
@@ -2517,8 +4004,12 @@
       <c r="N48">
         <v>106515</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -2561,8 +4052,12 @@
       <c r="N49">
         <v>106815</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2605,8 +4100,12 @@
       <c r="N50">
         <v>112435</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2649,8 +4148,12 @@
       <c r="N51">
         <v>116939</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4</v>
       </c>
@@ -2693,8 +4196,12 @@
       <c r="N52">
         <v>120075</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -2737,8 +4244,12 @@
       <c r="N53">
         <v>119179</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4</v>
       </c>
@@ -2781,8 +4292,12 @@
       <c r="N54">
         <v>121963</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4</v>
       </c>
@@ -2825,8 +4340,12 @@
       <c r="N55">
         <v>121629</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -2869,8 +4388,12 @@
       <c r="N56">
         <v>117599</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
@@ -2913,8 +4436,12 @@
       <c r="N57">
         <v>121590</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -2957,8 +4484,12 @@
       <c r="N58">
         <v>124416</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -3001,8 +4532,12 @@
       <c r="N59">
         <v>127721</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3045,8 +4580,12 @@
       <c r="N60">
         <v>128916</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3089,8 +4628,12 @@
       <c r="N61">
         <v>129886</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3133,8 +4676,12 @@
       <c r="N62">
         <v>143837</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4</v>
       </c>
@@ -3177,8 +4724,12 @@
       <c r="N63">
         <v>148472</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4</v>
       </c>
@@ -3221,8 +4772,12 @@
       <c r="N64">
         <v>151565</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4</v>
       </c>
@@ -3265,8 +4820,12 @@
       <c r="N65">
         <v>154686</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -3309,8 +4868,12 @@
       <c r="N66">
         <v>159273</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4</v>
       </c>
@@ -3352,6 +4915,101 @@
       </c>
       <c r="N67">
         <v>159921</v>
+      </c>
+      <c r="O67">
+        <f>IF(Table1[[#This Row],[Total]]&lt;&gt;"",MIN(IF(Table1[Nodes]=Table1[[#This Row],[Nodes]],IF(Table1[Problem size]=Table1[[#This Row],[Problem size]],Table1[Total]))))</f>
+        <v>94752</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>